<commit_message>
new draft after NHs comments
</commit_message>
<xml_diff>
--- a/data/categorization.xlsx
+++ b/data/categorization.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\git_projects\NH_luxation_infektion\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\NH_luxation_infektion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391D3A1E-A66A-47B4-867E-35BBD03F731B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="11520"/>
+    <workbookView xWindow="5805" yWindow="5805" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -107,9 +108,6 @@
     <t>moderate or severe liver disease</t>
   </si>
   <si>
-    <t>Lung airways disease</t>
-  </si>
-  <si>
     <t>chronic pulmonary disease</t>
   </si>
   <si>
@@ -384,12 +382,15 @@
   </si>
   <si>
     <t>antiplatelets</t>
+  </si>
+  <si>
+    <t>Lung and airways disease</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,11 +701,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,13 +717,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,7 +752,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -765,44 +766,44 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
         <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -818,10 +819,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,7 +846,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -859,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -872,20 +873,20 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,15 +915,15 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,15 +957,15 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,10 +989,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,31 +1021,31 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
         <v>27</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1052,65 +1053,65 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
         <v>30</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,76 +1119,76 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,34 +1196,34 @@
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
         <v>41</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
         <v>44</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1230,226 +1231,226 @@
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C80" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B90" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>